<commit_message>
Added function for soil dynamic properties and bugfix for soil profile creation from dataframes
</commit_message>
<xml_diff>
--- a/notebooks/Data/soilprofile_basic.xlsx
+++ b/notebooks/Data/soilprofile_basic.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/profound/Documents/Profound/Groundhog development/Output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/profound/Documents/SourceTree.tmp/ProFound/groundhog/notebooks/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A350EF-D445-6046-A13D-75CEAF8887E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7DADAD-8BBD-1449-BF3F-44CF9AF05171}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,12 +44,6 @@
     <t>SILT</t>
   </si>
   <si>
-    <t>z from [ft]</t>
-  </si>
-  <si>
-    <t>z to [ft]</t>
-  </si>
-  <si>
     <t>Relative density</t>
   </si>
   <si>
@@ -71,7 +65,13 @@
     <t>qt [MPa]</t>
   </si>
   <si>
-    <t>Subm unit weight [kN/m3]</t>
+    <t>Depth from [m]</t>
+  </si>
+  <si>
+    <t>Depth to [m]</t>
+  </si>
+  <si>
+    <t>Total unit weight [kN/m3]</t>
   </si>
 </sst>
 </file>
@@ -130,11 +130,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,42 +477,44 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -526,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -538,7 +541,7 @@
         <v>3.5</v>
       </c>
       <c r="H2">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -561,7 +564,7 @@
         <v>1.25</v>
       </c>
       <c r="H3">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -575,7 +578,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -587,7 +590,7 @@
         <v>6</v>
       </c>
       <c r="H4">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -601,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <v>40</v>
@@ -613,7 +616,7 @@
         <v>45</v>
       </c>
       <c r="H5">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>